<commit_message>
Chli doku mit bildli
</commit_message>
<xml_diff>
--- a/Files/Tabellen/Import-Evaluationsmatrix.xlsx
+++ b/Files/Tabellen/Import-Evaluationsmatrix.xlsx
@@ -210,16 +210,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -500,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -508,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,27 +522,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1">
@@ -564,7 +564,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1">
@@ -577,16 +577,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E6" si="0">B3*C3</f>
+        <f t="shared" ref="E3:E5" si="0">B3*C3</f>
         <v>28</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F6" si="1">D3*B3</f>
+        <f t="shared" ref="F3:F5" si="1">D3*B3</f>
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1">
@@ -608,99 +608,85 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="9">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="10">
         <v>10</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="4">
+        <f>SUM(C2:C5)</f>
+        <v>30</v>
+      </c>
+      <c r="D6" s="4">
+        <f>SUM(D2:D5)</f>
+        <v>23</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="5">
-        <f>SUM(C2:C6)</f>
-        <v>30</v>
-      </c>
-      <c r="D7" s="5">
-        <f>SUM(D2:D6)</f>
-        <v>23</v>
+      <c r="A7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="7">
+        <f>SUM(E2:E5)</f>
+        <v>88</v>
+      </c>
+      <c r="D7" s="4">
+        <f>SUM(F2:F5)</f>
+        <v>73</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="9">
-        <f>SUM(E2:E6)</f>
-        <v>88</v>
-      </c>
-      <c r="D8" s="5">
-        <f>SUM(F2:F6)</f>
-        <v>73</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>